<commit_message>
Watch main BOM progress.
</commit_message>
<xml_diff>
--- a/Documentation/BOMs/Watch Main BOM.xlsx
+++ b/Documentation/BOMs/Watch Main BOM.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bens1\Documents\Other\Projects\Smart-Watch\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bens1\Documents\Other\Projects\Smart-Watch\Documentation\BOMs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EF15490-ED02-4745-9015-9E7D45E1CE31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D74D49D-57EB-4854-89F8-42115FE829F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="114">
   <si>
     <t xml:space="preserve">DFE201612E-2R2M=P2 </t>
   </si>
@@ -342,6 +342,42 @@
   </si>
   <si>
     <t>nRF Regulator inductors</t>
+  </si>
+  <si>
+    <t>100nF, 0402</t>
+  </si>
+  <si>
+    <t>10uF, 0402</t>
+  </si>
+  <si>
+    <t>1uF, 0402</t>
+  </si>
+  <si>
+    <t>6pF, 0402</t>
+  </si>
+  <si>
+    <t>2.2uF, 0402</t>
+  </si>
+  <si>
+    <t>4.7uF, 0402</t>
+  </si>
+  <si>
+    <t>10nF, 0402</t>
+  </si>
+  <si>
+    <t>22uF, 0402</t>
+  </si>
+  <si>
+    <t>2.2nF, 0402</t>
+  </si>
+  <si>
+    <t>0.7pF, 0402</t>
+  </si>
+  <si>
+    <t>120pF, 0402</t>
+  </si>
+  <si>
+    <t>43pF</t>
   </si>
 </sst>
 </file>
@@ -683,11 +719,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J69"/>
+  <dimension ref="A1:J79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H22" sqref="H22"/>
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -695,7 +731,7 @@
     <col min="1" max="1" width="12.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="4" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="8.109375" customWidth="1"/>
     <col min="7" max="7" width="30.77734375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.6640625" style="2" bestFit="1" customWidth="1"/>
@@ -1001,295 +1037,382 @@
         <v>17</v>
       </c>
     </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>8</v>
+      </c>
+      <c r="B41" t="s">
+        <v>23</v>
+      </c>
+      <c r="C41" t="s">
+        <v>0</v>
+      </c>
+      <c r="D41" t="s">
+        <v>6</v>
+      </c>
+      <c r="E41">
+        <v>2</v>
+      </c>
+      <c r="F41" s="3">
+        <v>0.26</v>
+      </c>
+      <c r="G41" t="s">
+        <v>100</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="F42" s="3"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="F44" s="3"/>
+      <c r="C42" t="s">
+        <v>19</v>
+      </c>
+      <c r="D42" t="s">
+        <v>20</v>
+      </c>
+      <c r="E42">
+        <v>2</v>
+      </c>
+      <c r="F42" s="3">
+        <v>0.26</v>
+      </c>
+      <c r="G42" t="s">
+        <v>21</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C43" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D43" t="s">
+        <v>43</v>
+      </c>
+      <c r="E43">
+        <v>2</v>
+      </c>
+      <c r="F43" s="3">
+        <v>0.11</v>
+      </c>
+      <c r="G43" t="s">
+        <v>101</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="F45" s="3"/>
+      <c r="I45" s="1"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>8</v>
-      </c>
-      <c r="B46" t="s">
-        <v>23</v>
-      </c>
-      <c r="C46" t="s">
-        <v>0</v>
-      </c>
-      <c r="D46" t="s">
-        <v>6</v>
-      </c>
-      <c r="E46">
+      <c r="F46" s="3"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
+        <v>79</v>
+      </c>
+      <c r="C47" t="s">
+        <v>80</v>
+      </c>
+      <c r="D47" t="s">
+        <v>87</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
+      </c>
+      <c r="F47" s="3">
+        <v>0.54</v>
+      </c>
+      <c r="G47" t="s">
+        <v>81</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C48" t="s">
+        <v>85</v>
+      </c>
+      <c r="D48" t="s">
+        <v>84</v>
+      </c>
+      <c r="E48">
+        <v>1</v>
+      </c>
+      <c r="F48" s="3">
+        <v>0.32</v>
+      </c>
+      <c r="G48" t="s">
+        <v>83</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C49" t="s">
+        <v>91</v>
+      </c>
+      <c r="D49" t="s">
+        <v>89</v>
+      </c>
+      <c r="E49">
+        <v>1</v>
+      </c>
+      <c r="F49" s="3">
+        <v>0.37</v>
+      </c>
+      <c r="G49" t="s">
+        <v>90</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D51" t="s">
+        <v>111</v>
+      </c>
+      <c r="E51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D52" t="s">
+        <v>105</v>
+      </c>
+      <c r="E52">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D54" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="55" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D55" t="s">
+        <v>112</v>
+      </c>
+      <c r="E55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D56" t="s">
+        <v>110</v>
+      </c>
+      <c r="E56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D57" t="s">
+        <v>108</v>
+      </c>
+      <c r="E57">
         <v>2</v>
       </c>
-      <c r="F46" s="3">
-        <v>0.26</v>
-      </c>
-      <c r="G46" t="s">
-        <v>100</v>
-      </c>
-      <c r="I46" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C47" t="s">
-        <v>19</v>
-      </c>
-      <c r="D47" t="s">
-        <v>20</v>
-      </c>
-      <c r="E47">
+    </row>
+    <row r="58" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B58" t="s">
+        <v>95</v>
+      </c>
+      <c r="D58" t="s">
+        <v>102</v>
+      </c>
+      <c r="E58">
+        <v>36</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="59" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D59" t="s">
+        <v>104</v>
+      </c>
+      <c r="E59">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="60" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D60" t="s">
+        <v>106</v>
+      </c>
+      <c r="E60">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D61" t="s">
+        <v>107</v>
+      </c>
+      <c r="E61">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D62" t="s">
+        <v>103</v>
+      </c>
+      <c r="E62">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="63" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D63" t="s">
+        <v>109</v>
+      </c>
+      <c r="E63">
         <v>2</v>
       </c>
-      <c r="F47" s="3">
-        <v>0.26</v>
-      </c>
-      <c r="G47" t="s">
-        <v>21</v>
-      </c>
-      <c r="I47" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C48" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D48" t="s">
-        <v>43</v>
-      </c>
-      <c r="E48">
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F65" s="3"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C66" t="s">
+        <v>99</v>
+      </c>
+      <c r="D66" t="s">
+        <v>96</v>
+      </c>
+      <c r="E66">
         <v>2</v>
       </c>
-      <c r="F48" s="3">
-        <v>0.11</v>
-      </c>
-      <c r="G48" t="s">
-        <v>101</v>
-      </c>
-      <c r="I48" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="F50" s="3"/>
-      <c r="I50" s="1"/>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="F51" s="3"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B52" t="s">
-        <v>79</v>
-      </c>
-      <c r="C52" t="s">
-        <v>80</v>
-      </c>
-      <c r="D52" t="s">
-        <v>87</v>
-      </c>
-      <c r="E52">
-        <v>1</v>
-      </c>
-      <c r="F52" s="3">
-        <v>0.54</v>
-      </c>
-      <c r="G52" t="s">
-        <v>81</v>
-      </c>
-      <c r="I52" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C53" t="s">
-        <v>85</v>
-      </c>
-      <c r="D53" t="s">
-        <v>84</v>
-      </c>
-      <c r="E53">
-        <v>1</v>
-      </c>
-      <c r="F53" s="3">
-        <v>0.32</v>
-      </c>
-      <c r="G53" t="s">
-        <v>83</v>
-      </c>
-      <c r="I53" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C54" t="s">
-        <v>91</v>
-      </c>
-      <c r="D54" t="s">
-        <v>89</v>
-      </c>
-      <c r="E54">
-        <v>1</v>
-      </c>
-      <c r="F54" s="3">
-        <v>0.37</v>
-      </c>
-      <c r="G54" t="s">
-        <v>90</v>
-      </c>
-      <c r="I54" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="F55" s="3"/>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B56" t="s">
-        <v>95</v>
-      </c>
-      <c r="C56" t="s">
-        <v>99</v>
-      </c>
-      <c r="D56" t="s">
-        <v>96</v>
-      </c>
-      <c r="E56">
-        <v>2</v>
-      </c>
-      <c r="F56" s="3">
+      <c r="F66" s="3">
         <v>0.17699999999999999</v>
       </c>
-      <c r="G56" t="s">
+      <c r="G66" t="s">
         <v>98</v>
       </c>
-      <c r="I56" s="1" t="s">
+      <c r="I66" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="F57" s="3"/>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="F58" s="3"/>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F67" s="3"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F68" s="3"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
         <v>24</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B69" t="s">
         <v>25</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C69" t="s">
         <v>26</v>
       </c>
-      <c r="E59">
-        <v>1</v>
-      </c>
-      <c r="F59" s="3">
+      <c r="E69">
+        <v>1</v>
+      </c>
+      <c r="F69" s="3">
         <v>0.64</v>
       </c>
-      <c r="G59" t="s">
+      <c r="G69" t="s">
         <v>27</v>
       </c>
-      <c r="H59" s="2" t="s">
+      <c r="H69" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="I59" s="1" t="s">
+      <c r="I69" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B61" t="s">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B71" t="s">
         <v>49</v>
       </c>
-      <c r="C61" s="4"/>
-      <c r="E61">
-        <v>1</v>
-      </c>
-      <c r="G61" t="s">
+      <c r="C71" s="4"/>
+      <c r="E71">
+        <v>1</v>
+      </c>
+      <c r="G71" t="s">
         <v>50</v>
       </c>
-      <c r="I61" s="1"/>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C62" t="s">
+      <c r="I71" s="1"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C72" t="s">
         <v>58</v>
       </c>
-      <c r="E62">
-        <v>1</v>
-      </c>
-      <c r="F62">
+      <c r="E72">
+        <v>1</v>
+      </c>
+      <c r="F72">
         <v>0.82</v>
       </c>
-      <c r="G62" t="s">
+      <c r="G72" t="s">
         <v>59</v>
       </c>
-      <c r="I62" s="1" t="s">
+      <c r="I72" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C63" t="s">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C73" t="s">
         <v>62</v>
       </c>
-      <c r="E63">
-        <v>1</v>
-      </c>
-      <c r="F63" s="3">
+      <c r="E73">
+        <v>1</v>
+      </c>
+      <c r="F73" s="3">
         <v>1.4</v>
       </c>
-      <c r="G63" t="s">
+      <c r="G73" t="s">
         <v>73</v>
       </c>
-      <c r="I63" s="1" t="s">
+      <c r="I73" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C64" t="s">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C74" t="s">
         <v>72</v>
       </c>
-      <c r="E64">
-        <v>1</v>
-      </c>
-      <c r="F64" s="3">
+      <c r="E74">
+        <v>1</v>
+      </c>
+      <c r="F74" s="3">
         <v>2.04</v>
       </c>
-      <c r="G64" t="s">
+      <c r="G74" t="s">
         <v>74</v>
       </c>
-      <c r="I64" s="1" t="s">
+      <c r="I74" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="65" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F65" s="3"/>
-    </row>
-    <row r="66" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F66" s="3"/>
-    </row>
-    <row r="67" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F67" s="3"/>
-    </row>
-    <row r="68" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F68" s="3"/>
-    </row>
-    <row r="69" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F69" s="3"/>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F75" s="3"/>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F76" s="3"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F77" s="3"/>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F78" s="3"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F79" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="I46" r:id="rId1" xr:uid="{79C09E4D-BADE-4B4A-BEDF-E521AF2CD70D}"/>
+    <hyperlink ref="I41" r:id="rId1" xr:uid="{79C09E4D-BADE-4B4A-BEDF-E521AF2CD70D}"/>
     <hyperlink ref="I6" r:id="rId2" xr:uid="{F4A2A264-AC49-480B-919C-77721D13D06A}"/>
     <hyperlink ref="I39" r:id="rId3" xr:uid="{B2C0CAA1-46A0-4E27-9EB4-036D712BDB7E}"/>
-    <hyperlink ref="I47" r:id="rId4" xr:uid="{E042BE92-CD58-4075-A071-4B3A09485DEE}"/>
+    <hyperlink ref="I42" r:id="rId4" xr:uid="{E042BE92-CD58-4075-A071-4B3A09485DEE}"/>
     <hyperlink ref="I17" r:id="rId5" xr:uid="{A8D9A3BD-F369-470C-AD04-CFBD40E8EB05}"/>
     <hyperlink ref="I10" r:id="rId6" xr:uid="{923AFC17-08B1-4AD5-AB4A-F49FEEFA3BEC}"/>
     <hyperlink ref="I11" r:id="rId7" xr:uid="{C4894D1D-EE76-4C48-BCEF-A73F596BAA3D}"/>
@@ -1302,15 +1425,15 @@
     <hyperlink ref="I22" r:id="rId14" xr:uid="{D09DD33D-D05C-4448-9139-AD94F4FCFA1B}"/>
     <hyperlink ref="I3" r:id="rId15" xr:uid="{767704FF-C400-4F90-B6F1-9D33B5A14B1C}"/>
     <hyperlink ref="I4" r:id="rId16" xr:uid="{6C239A98-5AD8-44E7-8B22-0BEE5936F859}"/>
-    <hyperlink ref="I64" r:id="rId17" xr:uid="{DF11D2D2-F265-4769-80C5-92206328CB82}"/>
-    <hyperlink ref="I63" r:id="rId18" xr:uid="{8E26E8E6-7491-4A28-A0FC-173E24C5257D}"/>
-    <hyperlink ref="I62" r:id="rId19" xr:uid="{738C619A-46CB-4729-BF40-356AE1BA6342}"/>
-    <hyperlink ref="I59" r:id="rId20" xr:uid="{71B308CD-3568-4BEC-A754-5904C1F26182}"/>
-    <hyperlink ref="I56" r:id="rId21" xr:uid="{EC8C155B-E10F-41CA-941B-05D1EE3807A8}"/>
-    <hyperlink ref="I54" r:id="rId22" xr:uid="{C9E51835-D777-4C8A-8B6D-79598CB9D90D}"/>
-    <hyperlink ref="I53" r:id="rId23" xr:uid="{06406781-6B05-4280-99E0-2007222A2286}"/>
-    <hyperlink ref="I52" r:id="rId24" xr:uid="{3D0B6872-F586-4D57-B586-9244EB0BC9CA}"/>
-    <hyperlink ref="I48" r:id="rId25" xr:uid="{D440671E-DDBF-432C-9599-F06EDF3BD0EB}"/>
+    <hyperlink ref="I74" r:id="rId17" xr:uid="{DF11D2D2-F265-4769-80C5-92206328CB82}"/>
+    <hyperlink ref="I73" r:id="rId18" xr:uid="{8E26E8E6-7491-4A28-A0FC-173E24C5257D}"/>
+    <hyperlink ref="I72" r:id="rId19" xr:uid="{738C619A-46CB-4729-BF40-356AE1BA6342}"/>
+    <hyperlink ref="I69" r:id="rId20" xr:uid="{71B308CD-3568-4BEC-A754-5904C1F26182}"/>
+    <hyperlink ref="I66" r:id="rId21" xr:uid="{EC8C155B-E10F-41CA-941B-05D1EE3807A8}"/>
+    <hyperlink ref="I49" r:id="rId22" xr:uid="{C9E51835-D777-4C8A-8B6D-79598CB9D90D}"/>
+    <hyperlink ref="I48" r:id="rId23" xr:uid="{06406781-6B05-4280-99E0-2007222A2286}"/>
+    <hyperlink ref="I47" r:id="rId24" xr:uid="{3D0B6872-F586-4D57-B586-9244EB0BC9CA}"/>
+    <hyperlink ref="I43" r:id="rId25" xr:uid="{D440671E-DDBF-432C-9599-F06EDF3BD0EB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Created watch main board V3 Kicad project
</commit_message>
<xml_diff>
--- a/Documentation/BOMs/Watch Main BOM.xlsx
+++ b/Documentation/BOMs/Watch Main BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bens1\Documents\Other\Projects\Smart-Watch\Documentation\BOMs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bens1\OneDrive\Documents\Projects\Smart-Watch\Documentation\BOMs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF7CDD1-039A-4F2C-8A76-0E1683B1E9DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F828406-C563-4C22-90D3-361923EE0A37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-2970" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32985" yWindow="-16380" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="149">
   <si>
     <t xml:space="preserve">DFE201612E-2R2M=P2 </t>
   </si>
@@ -830,22 +830,22 @@
   <dimension ref="A1:J62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F62" sqref="F62"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H61" sqref="H61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="8.109375" customWidth="1"/>
-    <col min="7" max="7" width="33.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="8.140625" customWidth="1"/>
+    <col min="7" max="7" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.7109375" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>1</v>
       </c>
@@ -871,7 +871,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -894,7 +894,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>89</v>
       </c>
@@ -914,7 +914,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>12</v>
       </c>
@@ -934,7 +934,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>123</v>
       </c>
@@ -954,7 +954,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>126</v>
       </c>
@@ -974,7 +974,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>44</v>
       </c>
@@ -994,7 +994,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>36</v>
       </c>
@@ -1014,7 +1014,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>33</v>
       </c>
@@ -1034,7 +1034,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>38</v>
       </c>
@@ -1054,7 +1054,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>49</v>
       </c>
@@ -1074,7 +1074,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>53</v>
       </c>
@@ -1094,7 +1094,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>131</v>
       </c>
@@ -1114,7 +1114,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>30</v>
       </c>
@@ -1134,7 +1134,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>60</v>
       </c>
@@ -1154,7 +1154,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>68</v>
       </c>
@@ -1174,7 +1174,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>63</v>
       </c>
@@ -1194,7 +1194,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>52</v>
       </c>
@@ -1220,7 +1220,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -1240,7 +1240,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>133</v>
       </c>
@@ -1254,7 +1254,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>134</v>
       </c>
@@ -1268,7 +1268,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>135</v>
       </c>
@@ -1282,7 +1282,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>136</v>
       </c>
@@ -1296,7 +1296,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>0</v>
       </c>
@@ -1319,7 +1319,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
         <v>19</v>
       </c>
@@ -1342,7 +1342,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C29" s="4" t="s">
         <v>42</v>
       </c>
@@ -1365,12 +1365,12 @@
         <v>43</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C30" s="4"/>
       <c r="F30" s="3"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>76</v>
       </c>
@@ -1396,7 +1396,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
         <v>82</v>
       </c>
@@ -1419,7 +1419,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
         <v>88</v>
       </c>
@@ -1442,7 +1442,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>92</v>
       </c>
@@ -1459,7 +1459,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
         <v>137</v>
       </c>
@@ -1473,7 +1473,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
         <v>139</v>
       </c>
@@ -1487,7 +1487,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
         <v>140</v>
       </c>
@@ -1501,7 +1501,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
         <v>141</v>
       </c>
@@ -1515,7 +1515,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
         <v>142</v>
       </c>
@@ -1529,7 +1529,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
         <v>104</v>
       </c>
@@ -1540,7 +1540,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D42" t="s">
         <v>98</v>
       </c>
@@ -1551,7 +1551,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
         <v>143</v>
       </c>
@@ -1565,7 +1565,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D44" t="s">
         <v>100</v>
       </c>
@@ -1576,7 +1576,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D45" t="s">
         <v>102</v>
       </c>
@@ -1587,7 +1587,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D46" t="s">
         <v>103</v>
       </c>
@@ -1598,7 +1598,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D47" t="s">
         <v>99</v>
       </c>
@@ -1609,7 +1609,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
         <v>95</v>
       </c>
@@ -1632,7 +1632,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>113</v>
       </c>
@@ -1647,7 +1647,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D51" t="s">
         <v>112</v>
       </c>
@@ -1659,7 +1659,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C52" t="s">
         <v>144</v>
       </c>
@@ -1673,7 +1673,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D53" t="s">
         <v>115</v>
       </c>
@@ -1684,7 +1684,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>24</v>
       </c>
@@ -1710,7 +1710,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>47</v>
       </c>
@@ -1726,11 +1726,14 @@
       <c r="G57" t="s">
         <v>48</v>
       </c>
+      <c r="H57" s="2" t="s">
+        <v>132</v>
+      </c>
       <c r="I57" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C58" t="s">
         <v>56</v>
       </c>
@@ -1743,11 +1746,14 @@
       <c r="G58" t="s">
         <v>57</v>
       </c>
+      <c r="H58" s="2" t="s">
+        <v>132</v>
+      </c>
       <c r="I58" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C59" t="s">
         <v>59</v>
       </c>
@@ -1760,11 +1766,14 @@
       <c r="G59" t="s">
         <v>70</v>
       </c>
+      <c r="H59" s="2" t="s">
+        <v>132</v>
+      </c>
       <c r="I59" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C60" t="s">
         <v>69</v>
       </c>
@@ -1777,14 +1786,17 @@
       <c r="G60" t="s">
         <v>71</v>
       </c>
+      <c r="H60" s="2" t="s">
+        <v>132</v>
+      </c>
       <c r="I60" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F61" s="3"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F62" s="3"/>
     </row>
   </sheetData>
@@ -1817,6 +1829,8 @@
     <hyperlink ref="I7" r:id="rId25" xr:uid="{6683988D-DE60-4616-A3DC-FC7742914D6F}"/>
     <hyperlink ref="I14" r:id="rId26" xr:uid="{EC1B51B0-433F-4EF0-B5D2-CCA573C8B5F2}"/>
     <hyperlink ref="I15" r:id="rId27" xr:uid="{A8D9A3BD-F369-470C-AD04-CFBD40E8EB05}"/>
+    <hyperlink ref="I57" r:id="rId28" xr:uid="{D3CBBF69-5860-45BB-8944-6C7297A03CB8}"/>
+    <hyperlink ref="I58" r:id="rId29" xr:uid="{1F1BBFAF-D51B-4EBB-8CFA-16EC0569621C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Created touch connector footprint
</commit_message>
<xml_diff>
--- a/Documentation/BOMs/Watch Main BOM.xlsx
+++ b/Documentation/BOMs/Watch Main BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bens1\OneDrive\Documents\Projects\Smart-Watch\Documentation\BOMs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F828406-C563-4C22-90D3-361923EE0A37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD2B9837-B04F-4FF5-94C3-7EC44C455279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32985" yWindow="-16380" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2490" yWindow="1875" windowWidth="38700" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="150">
   <si>
     <t xml:space="preserve">DFE201612E-2R2M=P2 </t>
   </si>
@@ -483,6 +483,9 @@
   </si>
   <si>
     <t>https://www.digikey.co.uk/en/products/detail/molex/1051620001/4555282?s=N4IgTCBcDaIIwAYCscBsYC0DtxAXQF8g</t>
+  </si>
+  <si>
+    <t>WRONG</t>
   </si>
 </sst>
 </file>
@@ -830,8 +833,8 @@
   <dimension ref="A1:J62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H61" sqref="H61"/>
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1756,6 +1759,9 @@
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C59" t="s">
         <v>59</v>
+      </c>
+      <c r="D59" t="s">
+        <v>149</v>
       </c>
       <c r="E59">
         <v>1</v>

</xml_diff>